<commit_message>
Added sound to game. Added game logo.
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley\Desktop\FullSail\PG1\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanley\Desktop\FullSail\PG1\Pac-Man\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3948,23 +3948,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp174.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp175.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp176.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp177.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp178.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp179.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>